<commit_message>
:feature: [#0] obj dump dispaly
</commit_message>
<xml_diff>
--- a/doc/cpu_op.xlsx
+++ b/doc/cpu_op.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="135">
   <si>
     <t>opcode(8)</t>
   </si>
@@ -301,7 +301,7 @@
     <t>00000012</t>
   </si>
   <si>
-    <t>sll rs,rt,shamt</t>
+    <t>sll rs,rt</t>
   </si>
   <si>
     <r>
@@ -321,7 +321,7 @@
     <t>00000013</t>
   </si>
   <si>
-    <t>slr rs,rt,shamt</t>
+    <t>slr rs,rt</t>
   </si>
   <si>
     <r>
@@ -534,243 +534,313 @@
     <t>00000025</t>
   </si>
   <si>
+    <r>
+      <t>imm(16</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Droid Sans Fallback"/>
+        <charset val="134"/>
+      </rPr>
+      <t>位</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="DejaVu Sans Mono"/>
+        <charset val="134"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <t>lui rs, imm</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Droid Sans Fallback"/>
+        <charset val="134"/>
+      </rPr>
+      <t>将地址</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="DejaVu Sans Mono"/>
+        <charset val="134"/>
+      </rPr>
+      <t>imm</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Droid Sans Fallback"/>
+        <charset val="134"/>
+      </rPr>
+      <t>的的内存值，加载到</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="DejaVu Sans Mono"/>
+        <charset val="134"/>
+      </rPr>
+      <t>rs</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Droid Sans Fallback"/>
+        <charset val="134"/>
+      </rPr>
+      <t>里面</t>
+    </r>
+  </si>
+  <si>
+    <t>系统指令</t>
+  </si>
+  <si>
+    <t>00000026</t>
+  </si>
+  <si>
+    <t>call rs</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="DejaVu Sans"/>
+        <charset val="134"/>
+      </rPr>
+      <t>call rs</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Droid Sans Fallback"/>
+        <charset val="134"/>
+      </rPr>
+      <t>所代表的内存地址</t>
+    </r>
+  </si>
+  <si>
+    <t>00000027</t>
+  </si>
+  <si>
+    <t>calli imm</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="DejaVu Sans"/>
+        <charset val="134"/>
+      </rPr>
+      <t>call</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Droid Sans Fallback"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="DejaVu Sans"/>
+        <charset val="134"/>
+      </rPr>
+      <t>imm</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Droid Sans Fallback"/>
+        <charset val="134"/>
+      </rPr>
+      <t>所代表的内存地址</t>
+    </r>
+  </si>
+  <si>
+    <t>00000028</t>
+  </si>
+  <si>
+    <t>ret</t>
+  </si>
+  <si>
+    <t>返回调用</t>
+  </si>
+  <si>
+    <t>00000029</t>
+  </si>
+  <si>
+    <t>push rs</t>
+  </si>
+  <si>
+    <t>00000030</t>
+  </si>
+  <si>
+    <t>pop rs</t>
+  </si>
+  <si>
+    <t>00000031</t>
+  </si>
+  <si>
+    <r>
+      <t>imm</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Droid Sans Fallback"/>
+        <charset val="134"/>
+      </rPr>
+      <t>（</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="DejaVu Sans"/>
+        <charset val="134"/>
+      </rPr>
+      <t>8</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Droid Sans Fallback"/>
+        <charset val="134"/>
+      </rPr>
+      <t>位）</t>
+    </r>
+  </si>
+  <si>
+    <t>int imm</t>
+  </si>
+  <si>
+    <t>00000032</t>
+  </si>
+  <si>
+    <t>halt</t>
+  </si>
+  <si>
+    <t>停机</t>
+  </si>
+  <si>
+    <t>00000033</t>
+  </si>
+  <si>
+    <t>iret</t>
+  </si>
+  <si>
+    <t>00000034</t>
+  </si>
+  <si>
+    <t>lidt $label</t>
+  </si>
+  <si>
+    <t>加载中断描述符</t>
+  </si>
+  <si>
+    <t>00000035</t>
+  </si>
+  <si>
+    <t>num</t>
+  </si>
+  <si>
+    <t>lcr rs, num</t>
+  </si>
+  <si>
+    <r>
+      <t>加载</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="DejaVu Sans"/>
+        <charset val="134"/>
+      </rPr>
+      <t>cr0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Droid Sans Fallback"/>
+        <charset val="134"/>
+      </rPr>
+      <t>，</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="DejaVu Sans"/>
+        <charset val="134"/>
+      </rPr>
+      <t>cr1, cr2, cr3; cr0 = rs</t>
+    </r>
+  </si>
+  <si>
+    <t>00000036</t>
+  </si>
+  <si>
+    <t>sti</t>
+  </si>
+  <si>
+    <t>允许中断发生</t>
+  </si>
+  <si>
+    <t>00000037</t>
+  </si>
+  <si>
+    <t>cli</t>
+  </si>
+  <si>
+    <t>禁止中断发生</t>
+  </si>
+  <si>
+    <t>00000038</t>
+  </si>
+  <si>
+    <t>xor rs,rt,rd</t>
+  </si>
+  <si>
+    <t>rd = rs ^ rt</t>
+  </si>
+  <si>
+    <t>00000039</t>
+  </si>
+  <si>
     <t>imm</t>
   </si>
   <si>
-    <t>lui rs, imm</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Droid Sans Fallback"/>
-        <charset val="134"/>
-      </rPr>
-      <t>将地址</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="DejaVu Sans Mono"/>
-        <charset val="134"/>
-      </rPr>
-      <t>imm</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Droid Sans Fallback"/>
-        <charset val="134"/>
-      </rPr>
-      <t>的的内存值，加载到</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="DejaVu Sans Mono"/>
-        <charset val="134"/>
-      </rPr>
-      <t>rs</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Droid Sans Fallback"/>
-        <charset val="134"/>
-      </rPr>
-      <t>里面</t>
-    </r>
-  </si>
-  <si>
-    <t>系统指令</t>
-  </si>
-  <si>
-    <t>00000026</t>
-  </si>
-  <si>
-    <t>call rs</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="DejaVu Sans"/>
-        <charset val="134"/>
-      </rPr>
-      <t>call rs</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Droid Sans Fallback"/>
-        <charset val="134"/>
-      </rPr>
-      <t>所代表的内存地址</t>
-    </r>
-  </si>
-  <si>
-    <t>00000027</t>
-  </si>
-  <si>
-    <t>calli imm</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="DejaVu Sans"/>
-        <charset val="134"/>
-      </rPr>
-      <t>call</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Droid Sans Fallback"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="DejaVu Sans"/>
-        <charset val="134"/>
-      </rPr>
-      <t>imm</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Droid Sans Fallback"/>
-        <charset val="134"/>
-      </rPr>
-      <t>所代表的内存地址</t>
-    </r>
-  </si>
-  <si>
-    <t>00000028</t>
-  </si>
-  <si>
-    <t>ret</t>
-  </si>
-  <si>
-    <t>返回调用</t>
-  </si>
-  <si>
-    <t>00000029</t>
-  </si>
-  <si>
-    <t>push rs</t>
-  </si>
-  <si>
-    <t>00000030</t>
-  </si>
-  <si>
-    <t>pop rs</t>
-  </si>
-  <si>
-    <t>00000031</t>
-  </si>
-  <si>
-    <t>int imm</t>
-  </si>
-  <si>
-    <t>00000032</t>
-  </si>
-  <si>
-    <t>halt</t>
-  </si>
-  <si>
-    <t>停机</t>
-  </si>
-  <si>
-    <t>00000033</t>
-  </si>
-  <si>
-    <t>iret</t>
-  </si>
-  <si>
-    <t>00000034</t>
-  </si>
-  <si>
-    <t>lidt imm</t>
-  </si>
-  <si>
-    <t>加载中断描述符</t>
-  </si>
-  <si>
-    <t>00000035</t>
-  </si>
-  <si>
-    <t>lcr imm</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Droid Sans Fallback"/>
-        <charset val="134"/>
-      </rPr>
-      <t>加载</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="DejaVu Sans"/>
-        <charset val="134"/>
-      </rPr>
-      <t>cr0</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Droid Sans Fallback"/>
-        <charset val="134"/>
-      </rPr>
-      <t>，</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="DejaVu Sans"/>
-        <charset val="134"/>
-      </rPr>
-      <t>cr1, cr2, cr3</t>
-    </r>
-  </si>
-  <si>
-    <t>00000036</t>
-  </si>
-  <si>
-    <t>sti</t>
-  </si>
-  <si>
-    <t>允许中断发生</t>
-  </si>
-  <si>
-    <t>00000037</t>
-  </si>
-  <si>
-    <t>cli</t>
-  </si>
-  <si>
-    <t>禁止中断发生</t>
+    <t>addi rs,imm</t>
+  </si>
+  <si>
+    <t>rs = rs + imm</t>
   </si>
 </sst>
 </file>
@@ -972,7 +1042,7 @@
       <charset val="134"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -981,7 +1051,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1042,12 +1112,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1338,141 +1402,141 @@
     <xf numFmtId="0" fontId="21" fillId="10" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="32" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="28" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="33" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="18" fillId="31" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="21" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="29" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="27" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="25" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="32" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="19" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="22" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="17" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="28" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="24" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="23" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="18" fillId="30" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="14" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="26" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="18" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="29" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="31" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="15" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="27" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="12" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="10" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="11" applyNumberFormat="false" applyFont="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="9" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="9" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="6" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="15" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="5" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="13" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="12" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="9" borderId="10" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="11" applyNumberFormat="false" applyFont="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="9" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="9" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="6" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="16" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="5" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="14" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
@@ -1480,71 +1544,164 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="true" applyFill="true" applyBorder="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="true" applyFill="true" applyBorder="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="true" applyFill="true" applyBorder="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyFill="true" applyBorder="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="true" applyFill="true" applyBorder="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="left" vertical="top" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" quotePrefix="true">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="left" vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="true" applyFill="true" applyBorder="true" quotePrefix="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="true" applyFill="true" applyBorder="true" quotePrefix="true">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1866,881 +2023,926 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:G45"/>
+  <dimension ref="A1:G47"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" topLeftCell="A27" workbookViewId="0">
       <pane xSplit="1" topLeftCell="F1" activePane="topRight" state="frozen"/>
       <selection/>
-      <selection pane="topRight" activeCell="G17" sqref="G17"/>
+      <selection pane="topRight" activeCell="G48" sqref="G48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="15.75" outlineLevelCol="6"/>
   <cols>
     <col min="1" max="1" width="9.31333333333333" customWidth="true"/>
-    <col min="2" max="2" width="10.9533333333333" customWidth="true"/>
-    <col min="3" max="3" width="13.6733333333333" customWidth="true"/>
-    <col min="4" max="4" width="12.7066666666667" customWidth="true"/>
-    <col min="6" max="6" width="17.2" style="1" customWidth="true"/>
+    <col min="2" max="2" width="10.9533333333333" style="3" customWidth="true"/>
+    <col min="3" max="3" width="13.6733333333333" style="3" customWidth="true"/>
+    <col min="4" max="4" width="12.7066666666667" style="4" customWidth="true"/>
+    <col min="5" max="5" width="11.42" customWidth="true"/>
+    <col min="6" max="6" width="17.2" style="5" customWidth="true"/>
     <col min="7" max="7" width="35.1933333333333" customWidth="true"/>
   </cols>
   <sheetData>
-    <row r="1" ht="17.25" spans="1:7">
-      <c r="A1" s="2" t="s">
+    <row r="1" s="1" customFormat="true" ht="17.25" spans="1:7">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="14" t="s">
+      <c r="F1" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="35" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" ht="17.25" spans="1:7">
-      <c r="A2" s="4" t="s">
+    <row r="2" s="1" customFormat="true" ht="17.25" spans="1:7">
+      <c r="A2" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="15"/>
-      <c r="G2" s="5"/>
-    </row>
-    <row r="3" ht="17.25" spans="1:7">
-      <c r="A3" s="21" t="s">
+      <c r="B2" s="10"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="10"/>
+    </row>
+    <row r="3" s="2" customFormat="true" ht="17.25" spans="1:7">
+      <c r="A3" s="51" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="6" t="s">
+      <c r="B3" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="16" t="s">
+      <c r="F3" s="38" t="s">
         <v>13</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="G3" s="11" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="4" ht="17.25" spans="1:7">
-      <c r="A4" s="21" t="s">
+    <row r="4" s="2" customFormat="true" ht="17.25" spans="1:7">
+      <c r="A4" s="51" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="6" t="s">
+      <c r="B4" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D4" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E4" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="16" t="s">
+      <c r="F4" s="38" t="s">
         <v>16</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="G4" s="11" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="5" ht="17.25" spans="1:7">
-      <c r="A5" s="21" t="s">
+    <row r="5" s="2" customFormat="true" ht="17.25" spans="1:7">
+      <c r="A5" s="51" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="6" t="s">
+      <c r="B5" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="E5" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="F5" s="16" t="s">
+      <c r="F5" s="38" t="s">
         <v>19</v>
       </c>
-      <c r="G5" s="2" t="s">
+      <c r="G5" s="11" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="6" ht="17.25" spans="1:7">
-      <c r="A6" s="21" t="s">
+    <row r="6" s="2" customFormat="true" ht="17.25" spans="1:7">
+      <c r="A6" s="51" t="s">
         <v>21</v>
       </c>
-      <c r="B6" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" s="6" t="s">
+      <c r="B6" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="D6" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="E6" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="F6" s="16" t="s">
+      <c r="F6" s="38" t="s">
         <v>22</v>
       </c>
-      <c r="G6" s="2" t="s">
+      <c r="G6" s="11" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="7" ht="17.25" spans="1:7">
-      <c r="A7" s="21" t="s">
+    <row r="7" s="2" customFormat="true" ht="17.25" spans="1:7">
+      <c r="A7" s="51" t="s">
         <v>24</v>
       </c>
-      <c r="B7" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7" s="6" t="s">
+      <c r="B7" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="D7" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="E7" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="F7" s="16" t="s">
+      <c r="F7" s="38" t="s">
         <v>25</v>
       </c>
-      <c r="G7" s="2" t="s">
+      <c r="G7" s="11" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="8" ht="17.25" spans="1:7">
-      <c r="A8" s="4" t="s">
+    <row r="8" s="2" customFormat="true" ht="17.25" spans="1:7">
+      <c r="A8" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
-    </row>
-    <row r="9" ht="17.25" spans="1:7">
-      <c r="A9" s="21" t="s">
+      <c r="B8" s="14"/>
+      <c r="C8" s="14"/>
+      <c r="D8" s="14"/>
+      <c r="E8" s="14"/>
+      <c r="F8" s="14"/>
+      <c r="G8" s="14"/>
+    </row>
+    <row r="9" s="2" customFormat="true" ht="17.25" spans="1:7">
+      <c r="A9" s="51" t="s">
         <v>28</v>
       </c>
-      <c r="B9" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C9" s="2" t="s">
+      <c r="B9" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="D9" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="E9" s="2" t="s">
+      <c r="E9" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="F9" s="17" t="s">
+      <c r="F9" s="39" t="s">
         <v>30</v>
       </c>
-      <c r="G9" s="2" t="s">
+      <c r="G9" s="11" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="10" ht="17.25" spans="1:7">
-      <c r="A10" s="21" t="s">
+    <row r="10" s="2" customFormat="true" ht="17.25" spans="1:7">
+      <c r="A10" s="51" t="s">
         <v>31</v>
       </c>
-      <c r="B10" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C10" s="2" t="s">
+      <c r="B10" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="D10" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="E10" s="2" t="s">
+      <c r="E10" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="F10" s="17" t="s">
+      <c r="F10" s="39" t="s">
         <v>32</v>
       </c>
-      <c r="G10" s="2" t="s">
+      <c r="G10" s="11" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="11" ht="17.25" spans="1:7">
-      <c r="A11" s="21" t="s">
+    <row r="11" s="2" customFormat="true" ht="17.25" spans="1:7">
+      <c r="A11" s="51" t="s">
         <v>33</v>
       </c>
-      <c r="B11" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C11" s="2" t="s">
+      <c r="B11" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="D11" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="E11" s="2" t="s">
+      <c r="E11" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="F11" s="17" t="s">
+      <c r="F11" s="39" t="s">
         <v>34</v>
       </c>
-      <c r="G11" s="2" t="s">
+      <c r="G11" s="11" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="12" ht="17.25" spans="1:7">
-      <c r="A12" s="21" t="s">
+    <row r="12" s="2" customFormat="true" ht="17.25" spans="1:7">
+      <c r="A12" s="51" t="s">
         <v>35</v>
       </c>
-      <c r="B12" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C12" s="2" t="s">
+      <c r="B12" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="D12" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="E12" s="2" t="s">
+      <c r="E12" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="F12" s="17" t="s">
+      <c r="F12" s="39" t="s">
         <v>36</v>
       </c>
-      <c r="G12" s="2" t="s">
+      <c r="G12" s="11" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
-      <c r="A13" s="7" t="s">
+    <row r="13" s="2" customFormat="true" spans="1:7">
+      <c r="A13" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="B13" s="7"/>
-      <c r="C13" s="7"/>
-      <c r="D13" s="7"/>
-      <c r="E13" s="7"/>
-      <c r="F13" s="7"/>
-      <c r="G13" s="7"/>
-    </row>
-    <row r="14" ht="17.25" spans="1:7">
-      <c r="A14" s="21" t="s">
+      <c r="B13" s="17"/>
+      <c r="C13" s="17"/>
+      <c r="D13" s="17"/>
+      <c r="E13" s="17"/>
+      <c r="F13" s="17"/>
+      <c r="G13" s="17"/>
+    </row>
+    <row r="14" s="2" customFormat="true" ht="17.25" spans="1:7">
+      <c r="A14" s="51" t="s">
         <v>38</v>
       </c>
-      <c r="B14" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C14" s="2" t="s">
+      <c r="B14" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="D14" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="E14" s="2" t="s">
+      <c r="E14" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="F14" s="17" t="s">
+      <c r="F14" s="39" t="s">
         <v>39</v>
       </c>
-      <c r="G14" s="2" t="s">
+      <c r="G14" s="11" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="15" ht="17.25" spans="1:7">
-      <c r="A15" s="21" t="s">
+    <row r="15" s="2" customFormat="true" ht="17.25" spans="1:7">
+      <c r="A15" s="51" t="s">
         <v>41</v>
       </c>
-      <c r="B15" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C15" s="2" t="s">
+      <c r="B15" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="C15" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="D15" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="E15" s="2" t="s">
+      <c r="E15" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="F15" s="17" t="s">
+      <c r="F15" s="39" t="s">
         <v>42</v>
       </c>
-      <c r="G15" s="2" t="s">
+      <c r="G15" s="11" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="16" ht="17.25" spans="1:7">
-      <c r="A16" s="21" t="s">
+    <row r="16" s="2" customFormat="true" ht="17.25" spans="1:7">
+      <c r="A16" s="51" t="s">
         <v>44</v>
       </c>
-      <c r="B16" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C16" s="2" t="s">
+      <c r="B16" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="C16" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="D16" s="4" t="s">
+      <c r="D16" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="E16" s="8"/>
-      <c r="F16" s="17" t="s">
+      <c r="E16" s="20"/>
+      <c r="F16" s="39" t="s">
         <v>46</v>
       </c>
-      <c r="G16" s="2" t="s">
+      <c r="G16" s="11" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="17" ht="17.25" spans="1:7">
-      <c r="A17" s="21" t="s">
+    <row r="17" s="2" customFormat="true" ht="17.25" spans="1:7">
+      <c r="A17" s="51" t="s">
         <v>48</v>
       </c>
-      <c r="B17" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C17" s="2" t="s">
+      <c r="B17" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="C17" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="D17" s="4" t="s">
+      <c r="D17" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="E17" s="8"/>
-      <c r="F17" s="17" t="s">
+      <c r="E17" s="20"/>
+      <c r="F17" s="39" t="s">
         <v>49</v>
       </c>
-      <c r="G17" s="2" t="s">
+      <c r="G17" s="11" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="18" ht="17.25" spans="1:7">
-      <c r="A18" s="21" t="s">
+    <row r="18" s="2" customFormat="true" ht="17.25" spans="1:7">
+      <c r="A18" s="51" t="s">
         <v>51</v>
       </c>
-      <c r="B18" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C18" s="2" t="s">
+      <c r="B18" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="C18" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="D18" s="4" t="s">
+      <c r="D18" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="E18" s="8"/>
-      <c r="F18" s="17" t="s">
+      <c r="E18" s="20"/>
+      <c r="F18" s="39" t="s">
         <v>52</v>
       </c>
-      <c r="G18" s="2" t="s">
+      <c r="G18" s="11" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="19" spans="1:7">
-      <c r="A19" s="7" t="s">
+    <row r="19" s="1" customFormat="true" spans="1:7">
+      <c r="A19" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="B19" s="7"/>
-      <c r="C19" s="7"/>
-      <c r="D19" s="7"/>
-      <c r="E19" s="7"/>
-      <c r="F19" s="7"/>
-      <c r="G19" s="7"/>
-    </row>
-    <row r="20" spans="1:7">
-      <c r="A20" s="21" t="s">
+      <c r="B19" s="18"/>
+      <c r="C19" s="18"/>
+      <c r="D19" s="18"/>
+      <c r="E19" s="18"/>
+      <c r="F19" s="18"/>
+      <c r="G19" s="18"/>
+    </row>
+    <row r="20" s="2" customFormat="true" spans="1:7">
+      <c r="A20" s="51" t="s">
         <v>55</v>
       </c>
-      <c r="B20" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C20" s="2" t="s">
+      <c r="B20" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="C20" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="D20" s="8" t="s">
+      <c r="D20" s="19" t="s">
         <v>56</v>
       </c>
-      <c r="E20" s="8"/>
-      <c r="F20" s="17" t="s">
+      <c r="E20" s="19"/>
+      <c r="F20" s="39" t="s">
         <v>57</v>
       </c>
-      <c r="G20" s="2" t="s">
+      <c r="G20" s="11" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="21" spans="1:7">
-      <c r="A21" s="21" t="s">
+    <row r="21" s="2" customFormat="true" spans="1:7">
+      <c r="A21" s="51" t="s">
         <v>59</v>
       </c>
-      <c r="B21" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C21" s="2" t="s">
+      <c r="B21" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="C21" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="D21" s="8" t="s">
+      <c r="D21" s="19" t="s">
         <v>56</v>
       </c>
-      <c r="E21" s="8"/>
-      <c r="F21" s="17" t="s">
+      <c r="E21" s="19"/>
+      <c r="F21" s="39" t="s">
         <v>60</v>
       </c>
-      <c r="G21" s="2" t="s">
+      <c r="G21" s="11" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="22" spans="1:7">
-      <c r="A22" s="21" t="s">
+    <row r="22" s="2" customFormat="true" spans="1:7">
+      <c r="A22" s="51" t="s">
         <v>62</v>
       </c>
-      <c r="B22" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C22" s="2" t="s">
+      <c r="B22" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="C22" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="D22" s="8" t="s">
+      <c r="D22" s="19" t="s">
         <v>56</v>
       </c>
-      <c r="E22" s="8"/>
-      <c r="F22" s="17" t="s">
+      <c r="E22" s="19"/>
+      <c r="F22" s="39" t="s">
         <v>63</v>
       </c>
-      <c r="G22" s="2" t="s">
+      <c r="G22" s="11" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="23" spans="1:7">
-      <c r="A23" s="21" t="s">
+    <row r="23" s="2" customFormat="true" spans="1:7">
+      <c r="A23" s="51" t="s">
         <v>65</v>
       </c>
-      <c r="B23" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C23" s="2" t="s">
+      <c r="B23" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="C23" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="D23" s="8" t="s">
+      <c r="D23" s="19" t="s">
         <v>56</v>
       </c>
-      <c r="E23" s="8"/>
-      <c r="F23" s="17" t="s">
+      <c r="E23" s="19"/>
+      <c r="F23" s="39" t="s">
         <v>66</v>
       </c>
-      <c r="G23" s="2" t="s">
+      <c r="G23" s="11" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="24" spans="1:7">
-      <c r="A24" s="21" t="s">
+    <row r="24" s="2" customFormat="true" spans="1:7">
+      <c r="A24" s="51" t="s">
         <v>68</v>
       </c>
-      <c r="B24" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C24" s="2" t="s">
+      <c r="B24" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="C24" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="D24" s="8" t="s">
+      <c r="D24" s="19" t="s">
         <v>56</v>
       </c>
-      <c r="E24" s="8"/>
-      <c r="F24" s="17" t="s">
+      <c r="E24" s="19"/>
+      <c r="F24" s="39" t="s">
         <v>69</v>
       </c>
-      <c r="G24" s="2" t="s">
+      <c r="G24" s="11" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="25" spans="1:7">
-      <c r="A25" s="21" t="s">
+    <row r="25" s="2" customFormat="true" spans="1:7">
+      <c r="A25" s="51" t="s">
         <v>71</v>
       </c>
-      <c r="B25" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C25" s="2" t="s">
+      <c r="B25" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="C25" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="D25" s="8" t="s">
+      <c r="D25" s="19" t="s">
         <v>56</v>
       </c>
-      <c r="E25" s="8"/>
-      <c r="F25" s="17" t="s">
+      <c r="E25" s="19"/>
+      <c r="F25" s="39" t="s">
         <v>72</v>
       </c>
-      <c r="G25" s="2" t="s">
+      <c r="G25" s="11" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="26" ht="17.25" spans="1:7">
-      <c r="A26" s="21" t="s">
+    <row r="26" s="2" customFormat="true" ht="17.25" spans="1:7">
+      <c r="A26" s="51" t="s">
         <v>74</v>
       </c>
-      <c r="B26" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C26" s="4" t="s">
+      <c r="B26" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="C26" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="D26" s="8"/>
-      <c r="E26" s="8"/>
-      <c r="F26" s="17" t="s">
+      <c r="D26" s="20"/>
+      <c r="E26" s="20"/>
+      <c r="F26" s="39" t="s">
         <v>75</v>
       </c>
-      <c r="G26" s="2" t="s">
+      <c r="G26" s="11" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="27" spans="1:7">
-      <c r="A27" s="21" t="s">
+    <row r="27" s="2" customFormat="true" spans="1:7">
+      <c r="A27" s="51" t="s">
         <v>76</v>
       </c>
-      <c r="B27" s="8" t="s">
+      <c r="B27" s="19" t="s">
         <v>56</v>
       </c>
-      <c r="C27" s="8"/>
-      <c r="D27" s="8"/>
-      <c r="E27" s="8"/>
-      <c r="F27" s="17" t="s">
+      <c r="C27" s="19"/>
+      <c r="D27" s="19"/>
+      <c r="E27" s="19"/>
+      <c r="F27" s="39" t="s">
         <v>77</v>
       </c>
-      <c r="G27" s="2" t="s">
+      <c r="G27" s="11" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="28" spans="1:7">
-      <c r="A28" s="9" t="s">
+    <row r="28" s="1" customFormat="true" spans="1:7">
+      <c r="A28" s="21" t="s">
         <v>79</v>
       </c>
-      <c r="B28" s="9"/>
-      <c r="C28" s="9"/>
-      <c r="D28" s="9"/>
-      <c r="E28" s="9"/>
-      <c r="F28" s="9"/>
-      <c r="G28" s="9"/>
-    </row>
-    <row r="29" ht="17.25" spans="1:7">
-      <c r="A29" s="21" t="s">
+      <c r="B28" s="21"/>
+      <c r="C28" s="21"/>
+      <c r="D28" s="21"/>
+      <c r="E28" s="21"/>
+      <c r="F28" s="21"/>
+      <c r="G28" s="21"/>
+    </row>
+    <row r="29" s="2" customFormat="true" ht="17.25" spans="1:7">
+      <c r="A29" s="51" t="s">
         <v>80</v>
       </c>
-      <c r="B29" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C29" s="2" t="s">
+      <c r="B29" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="C29" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="D29" s="4" t="s">
+      <c r="D29" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="E29" s="8"/>
-      <c r="F29" s="17" t="s">
+      <c r="E29" s="20"/>
+      <c r="F29" s="39" t="s">
         <v>81</v>
       </c>
-      <c r="G29" s="2" t="s">
+      <c r="G29" s="11" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="30" ht="17.25" spans="1:7">
-      <c r="A30" s="21" t="s">
+    <row r="30" s="2" customFormat="true" ht="17.25" spans="1:7">
+      <c r="A30" s="51" t="s">
         <v>83</v>
       </c>
-      <c r="B30" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C30" s="2" t="s">
+      <c r="B30" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="C30" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="D30" s="4" t="s">
+      <c r="D30" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="E30" s="8"/>
-      <c r="F30" s="17" t="s">
+      <c r="E30" s="20"/>
+      <c r="F30" s="39" t="s">
         <v>84</v>
       </c>
-      <c r="G30" s="2" t="s">
+      <c r="G30" s="11" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="31" ht="17.25" spans="1:7">
-      <c r="A31" s="21" t="s">
+    <row r="31" s="2" customFormat="true" ht="17.25" spans="1:7">
+      <c r="A31" s="51" t="s">
         <v>86</v>
       </c>
-      <c r="B31" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C31" s="2" t="s">
+      <c r="B31" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="C31" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="D31" s="4" t="s">
+      <c r="D31" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="E31" s="8"/>
-      <c r="F31" s="17" t="s">
+      <c r="E31" s="20"/>
+      <c r="F31" s="39" t="s">
         <v>87</v>
       </c>
-      <c r="G31" s="2" t="s">
+      <c r="G31" s="11" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="32" ht="17.25" spans="1:7">
-      <c r="A32" s="21" t="s">
+    <row r="32" s="1" customFormat="true" ht="17.25" spans="1:7">
+      <c r="A32" s="52" t="s">
         <v>89</v>
       </c>
-      <c r="B32" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C32" s="10" t="s">
+      <c r="B32" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="C32" s="23" t="s">
         <v>90</v>
       </c>
-      <c r="D32" s="11"/>
-      <c r="E32" s="18"/>
-      <c r="F32" s="17" t="s">
+      <c r="D32" s="24"/>
+      <c r="E32" s="40"/>
+      <c r="F32" s="41" t="s">
         <v>91</v>
       </c>
-      <c r="G32" s="3" t="s">
+      <c r="G32" s="35" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="33" spans="1:7">
-      <c r="A33" s="9" t="s">
+    <row r="33" s="1" customFormat="true" spans="1:7">
+      <c r="A33" s="21" t="s">
         <v>93</v>
       </c>
-      <c r="B33" s="9"/>
-      <c r="C33" s="9"/>
-      <c r="D33" s="9"/>
-      <c r="E33" s="9"/>
-      <c r="F33" s="9"/>
-      <c r="G33" s="9"/>
-    </row>
-    <row r="34" ht="17.25" spans="1:7">
-      <c r="A34" s="21" t="s">
+      <c r="B33" s="21"/>
+      <c r="C33" s="21"/>
+      <c r="D33" s="21"/>
+      <c r="E33" s="21"/>
+      <c r="F33" s="21"/>
+      <c r="G33" s="21"/>
+    </row>
+    <row r="34" s="2" customFormat="true" ht="17.25" spans="1:7">
+      <c r="A34" s="51" t="s">
         <v>94</v>
       </c>
-      <c r="B34" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C34" s="12" t="s">
+      <c r="B34" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="C34" s="25" t="s">
         <v>45</v>
       </c>
-      <c r="D34" s="11"/>
-      <c r="E34" s="18"/>
-      <c r="F34" s="17" t="s">
+      <c r="D34" s="26"/>
+      <c r="E34" s="42"/>
+      <c r="F34" s="39" t="s">
         <v>95</v>
       </c>
-      <c r="G34" s="19" t="s">
+      <c r="G34" s="43" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="35" ht="17.25" spans="1:7">
-      <c r="A35" s="21" t="s">
+    <row r="35" s="2" customFormat="true" ht="17.25" spans="1:7">
+      <c r="A35" s="51" t="s">
         <v>97</v>
       </c>
-      <c r="B35" s="10" t="s">
-        <v>90</v>
-      </c>
-      <c r="C35" s="11"/>
-      <c r="D35" s="11"/>
-      <c r="E35" s="18"/>
-      <c r="F35" s="17" t="s">
+      <c r="B35" s="27" t="s">
+        <v>56</v>
+      </c>
+      <c r="C35" s="28"/>
+      <c r="D35" s="28"/>
+      <c r="E35" s="44"/>
+      <c r="F35" s="39" t="s">
         <v>98</v>
       </c>
-      <c r="G35" s="19" t="s">
+      <c r="G35" s="43" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="36" ht="17.25" spans="1:7">
-      <c r="A36" s="21" t="s">
+    <row r="36" s="2" customFormat="true" ht="17.25" spans="1:7">
+      <c r="A36" s="51" t="s">
         <v>100</v>
       </c>
-      <c r="B36" s="12" t="s">
+      <c r="B36" s="25" t="s">
         <v>45</v>
       </c>
-      <c r="C36" s="11"/>
-      <c r="D36" s="11"/>
-      <c r="E36" s="18"/>
-      <c r="F36" s="17" t="s">
+      <c r="C36" s="26"/>
+      <c r="D36" s="26"/>
+      <c r="E36" s="42"/>
+      <c r="F36" s="39" t="s">
         <v>101</v>
       </c>
-      <c r="G36" s="3" t="s">
+      <c r="G36" s="45" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="37" ht="17.25" spans="1:7">
-      <c r="A37" s="21" t="s">
+    <row r="37" s="2" customFormat="true" ht="17.25" spans="1:7">
+      <c r="A37" s="51" t="s">
         <v>103</v>
       </c>
-      <c r="B37" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C37" s="12" t="s">
+      <c r="B37" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="C37" s="25" t="s">
         <v>45</v>
       </c>
-      <c r="D37" s="11"/>
-      <c r="E37" s="18"/>
-      <c r="F37" s="20" t="s">
+      <c r="D37" s="26"/>
+      <c r="E37" s="42"/>
+      <c r="F37" s="46" t="s">
         <v>104</v>
       </c>
-      <c r="G37" s="3"/>
-    </row>
-    <row r="38" ht="17.25" spans="1:7">
-      <c r="A38" s="21" t="s">
+      <c r="G37" s="45"/>
+    </row>
+    <row r="38" s="2" customFormat="true" ht="17.25" spans="1:7">
+      <c r="A38" s="51" t="s">
         <v>105</v>
       </c>
-      <c r="B38" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C38" s="12" t="s">
+      <c r="B38" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="C38" s="25" t="s">
         <v>45</v>
       </c>
-      <c r="D38" s="11"/>
-      <c r="E38" s="18"/>
-      <c r="F38" s="17" t="s">
+      <c r="D38" s="26"/>
+      <c r="E38" s="42"/>
+      <c r="F38" s="39" t="s">
         <v>106</v>
       </c>
-      <c r="G38" s="3"/>
-    </row>
-    <row r="39" ht="17.25" spans="1:7">
-      <c r="A39" s="21" t="s">
+      <c r="G38" s="45"/>
+    </row>
+    <row r="39" s="1" customFormat="true" ht="17.25" spans="1:7">
+      <c r="A39" s="52" t="s">
         <v>107</v>
       </c>
-      <c r="B39" s="13" t="s">
-        <v>90</v>
-      </c>
-      <c r="C39" s="12" t="s">
+      <c r="B39" s="29" t="s">
         <v>45</v>
       </c>
-      <c r="D39" s="11"/>
-      <c r="E39" s="18"/>
-      <c r="F39" s="17" t="s">
+      <c r="C39" s="30"/>
+      <c r="D39" s="30"/>
+      <c r="E39" s="47" t="s">
         <v>108</v>
       </c>
-      <c r="G39" s="3"/>
-    </row>
-    <row r="40" ht="17.25" spans="1:7">
-      <c r="A40" s="21" t="s">
+      <c r="F39" s="41" t="s">
         <v>109</v>
       </c>
-      <c r="B40" s="12" t="s">
+      <c r="G39" s="35"/>
+    </row>
+    <row r="40" s="2" customFormat="true" ht="17.25" spans="1:7">
+      <c r="A40" s="51" t="s">
+        <v>110</v>
+      </c>
+      <c r="B40" s="25" t="s">
         <v>45</v>
       </c>
-      <c r="C40" s="11"/>
-      <c r="D40" s="11"/>
-      <c r="E40" s="18"/>
-      <c r="F40" s="17" t="s">
-        <v>110</v>
-      </c>
-      <c r="G40" s="3" t="s">
+      <c r="C40" s="26"/>
+      <c r="D40" s="26"/>
+      <c r="E40" s="42"/>
+      <c r="F40" s="39" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="41" ht="17.25" spans="1:7">
-      <c r="A41" s="21" t="s">
+      <c r="G40" s="45" t="s">
         <v>112</v>
       </c>
-      <c r="B41" s="12" t="s">
+    </row>
+    <row r="41" s="2" customFormat="true" ht="17.25" spans="1:7">
+      <c r="A41" s="51" t="s">
+        <v>113</v>
+      </c>
+      <c r="B41" s="25" t="s">
         <v>45</v>
       </c>
-      <c r="C41" s="11"/>
-      <c r="D41" s="11"/>
-      <c r="E41" s="18"/>
-      <c r="F41" s="20" t="s">
-        <v>113</v>
-      </c>
-      <c r="G41" s="3"/>
-    </row>
-    <row r="42" ht="17.25" spans="1:7">
-      <c r="A42" s="21" t="s">
+      <c r="C41" s="26"/>
+      <c r="D41" s="26"/>
+      <c r="E41" s="42"/>
+      <c r="F41" s="46" t="s">
         <v>114</v>
       </c>
-      <c r="B42" s="12" t="s">
-        <v>90</v>
-      </c>
-      <c r="C42" s="11"/>
-      <c r="D42" s="11"/>
-      <c r="E42" s="18"/>
-      <c r="F42" s="20" t="s">
+      <c r="G41" s="45"/>
+    </row>
+    <row r="42" s="2" customFormat="true" ht="17.25" spans="1:7">
+      <c r="A42" s="51" t="s">
         <v>115</v>
       </c>
-      <c r="G42" s="3" t="s">
+      <c r="B42" s="31" t="s">
+        <v>56</v>
+      </c>
+      <c r="C42" s="28"/>
+      <c r="D42" s="28"/>
+      <c r="E42" s="44"/>
+      <c r="F42" s="46" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="43" ht="17.25" spans="1:7">
-      <c r="A43" s="21" t="s">
+      <c r="G42" s="45" t="s">
         <v>117</v>
       </c>
-      <c r="B43" s="13" t="s">
-        <v>90</v>
-      </c>
-      <c r="C43" s="12" t="s">
+    </row>
+    <row r="43" s="1" customFormat="true" ht="17.25" spans="1:7">
+      <c r="A43" s="52" t="s">
+        <v>118</v>
+      </c>
+      <c r="B43" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="C43" s="32" t="s">
+        <v>119</v>
+      </c>
+      <c r="D43" s="30" t="s">
         <v>45</v>
       </c>
-      <c r="D43" s="11"/>
-      <c r="E43" s="18"/>
-      <c r="F43" s="20" t="s">
-        <v>118</v>
-      </c>
-      <c r="G43" s="3" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="44" ht="17.25" spans="1:7">
-      <c r="A44" s="21" t="s">
+      <c r="E43" s="48"/>
+      <c r="F43" s="49" t="s">
         <v>120</v>
       </c>
-      <c r="B44" s="12" t="s">
+      <c r="G43" s="35" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="44" s="2" customFormat="true" ht="17.25" spans="1:7">
+      <c r="A44" s="51" t="s">
+        <v>122</v>
+      </c>
+      <c r="B44" s="25" t="s">
         <v>45</v>
       </c>
-      <c r="C44" s="11"/>
-      <c r="D44" s="11"/>
-      <c r="E44" s="18"/>
-      <c r="F44" s="20" t="s">
-        <v>121</v>
-      </c>
-      <c r="G44" s="3" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="45" ht="17.25" spans="1:7">
-      <c r="A45" s="21" t="s">
+      <c r="C44" s="26"/>
+      <c r="D44" s="26"/>
+      <c r="E44" s="42"/>
+      <c r="F44" s="46" t="s">
         <v>123</v>
       </c>
-      <c r="B45" s="12" t="s">
+      <c r="G44" s="45" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="45" s="2" customFormat="true" ht="17.25" spans="1:7">
+      <c r="A45" s="51" t="s">
+        <v>125</v>
+      </c>
+      <c r="B45" s="25" t="s">
         <v>45</v>
       </c>
-      <c r="C45" s="11"/>
-      <c r="D45" s="11"/>
-      <c r="E45" s="18"/>
-      <c r="F45" s="20" t="s">
-        <v>124</v>
-      </c>
-      <c r="G45" s="3" t="s">
-        <v>125</v>
+      <c r="C45" s="26"/>
+      <c r="D45" s="26"/>
+      <c r="E45" s="42"/>
+      <c r="F45" s="46" t="s">
+        <v>126</v>
+      </c>
+      <c r="G45" s="45" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="46" s="2" customFormat="true" ht="17.25" spans="1:7">
+      <c r="A46" s="51" t="s">
+        <v>128</v>
+      </c>
+      <c r="B46" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="C46" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="D46" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="E46" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="F46" s="39" t="s">
+        <v>129</v>
+      </c>
+      <c r="G46" s="11" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="47" s="2" customFormat="true" ht="17.25" spans="1:7">
+      <c r="A47" s="51" t="s">
+        <v>131</v>
+      </c>
+      <c r="B47" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="C47" s="33" t="s">
+        <v>132</v>
+      </c>
+      <c r="D47" s="34"/>
+      <c r="E47" s="50"/>
+      <c r="F47" s="39" t="s">
+        <v>133</v>
+      </c>
+      <c r="G47" s="11" t="s">
+        <v>134</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="33">
+  <mergeCells count="34">
     <mergeCell ref="A2:G2"/>
     <mergeCell ref="A8:G8"/>
     <mergeCell ref="A13:G13"/>
@@ -2767,13 +2969,14 @@
     <mergeCell ref="B36:E36"/>
     <mergeCell ref="C37:E37"/>
     <mergeCell ref="C38:E38"/>
-    <mergeCell ref="C39:E39"/>
+    <mergeCell ref="B39:D39"/>
     <mergeCell ref="B40:E40"/>
     <mergeCell ref="B41:E41"/>
     <mergeCell ref="B42:E42"/>
-    <mergeCell ref="C43:E43"/>
+    <mergeCell ref="D43:E43"/>
     <mergeCell ref="B44:E44"/>
     <mergeCell ref="B45:E45"/>
+    <mergeCell ref="C47:E47"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>